<commit_message>
pcb: Corrections to BOM
</commit_message>
<xml_diff>
--- a/pcb/BOM.xlsx
+++ b/pcb/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhiyb\Documents\Design\embedded\Nosumor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhiyb\Documents\Design\embedded\Nosumor\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="180">
   <si>
     <t>Type</t>
   </si>
@@ -104,9 +104,6 @@
     <t>C7</t>
   </si>
   <si>
-    <t>C2, C12, C13, C15, C16, C18</t>
-  </si>
-  <si>
     <t>18p</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>D4, D6</t>
   </si>
   <si>
-    <t>150</t>
-  </si>
-  <si>
     <t>R2, R4, R6</t>
   </si>
   <si>
@@ -227,9 +221,6 @@
     <t>Cherry-MX</t>
   </si>
   <si>
-    <t>K1, K2</t>
-  </si>
-  <si>
     <t>Tactile</t>
   </si>
   <si>
@@ -564,6 +555,15 @@
   </si>
   <si>
     <t>AliExpress</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C2, C12, C13, C15, C16</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -571,7 +571,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="&quot;£&quot;#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -611,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -625,7 +625,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -633,7 +634,7 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="172" formatCode="&quot;£&quot;#,##0.000"/>
+      <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.000"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -642,7 +643,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="&quot;£&quot;#,##0.000"/>
+      <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -676,12 +677,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A4B88EC-684F-4D5A-8F53-23ADBD7DDE28}" name="Table3" displayName="Table3" ref="A1:H50" totalsRowCount="1" headerRowDxfId="9">
-  <autoFilter ref="A1:H49" xr:uid="{C6C29A0C-1C9D-4BBE-AA50-69AB5F03B3F7}"/>
-  <sortState ref="A2:H49">
-    <sortCondition ref="A2:A49"/>
-    <sortCondition ref="B2:B49"/>
-    <sortCondition descending="1" ref="F2:F49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A4B88EC-684F-4D5A-8F53-23ADBD7DDE28}" name="Table3" displayName="Table3" ref="A1:H51" totalsRowCount="1" headerRowDxfId="9">
+  <autoFilter ref="A1:H50" xr:uid="{C6C29A0C-1C9D-4BBE-AA50-69AB5F03B3F7}"/>
+  <sortState ref="A2:H50">
+    <sortCondition ref="A2:A50"/>
+    <sortCondition ref="B2:B50"/>
+    <sortCondition descending="1" ref="F2:F50"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{52C12E02-52FF-4249-B643-36E1BF14DE4D}" name="Section" totalsRowLabel="Total" dataDxfId="8"/>
@@ -998,11 +999,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1038,7 @@
         <v>22</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -1054,7 +1055,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>18</v>
@@ -1067,7 +1068,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1078,13 +1079,13 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="E3" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F3" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1094,7 +1095,7 @@
         <v>0.29399999999999998</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1105,13 +1106,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F4" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1121,7 +1122,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1132,13 +1133,13 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F5" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1148,7 +1149,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1159,13 +1160,13 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F6" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1175,7 +1176,7 @@
         <v>2.3E-2</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1186,13 +1187,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F7" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1202,7 +1203,7 @@
         <v>0.81100000000000005</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1213,13 +1214,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F8" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1229,7 +1230,7 @@
         <v>0.25</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1240,13 +1241,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F9" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1256,7 +1257,7 @@
         <v>4.01</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1267,13 +1268,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F10" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1283,7 +1284,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1294,13 +1295,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F11" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1310,7 +1311,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1324,7 +1325,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>18</v>
@@ -1337,7 +1338,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1348,13 +1349,13 @@
         <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F13" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1364,7 +1365,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1375,13 +1376,13 @@
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F14" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1391,7 +1392,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1402,13 +1403,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F15" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1418,7 +1419,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1429,13 +1430,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F16" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1445,7 +1446,7 @@
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1456,13 +1457,13 @@
         <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F17" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1472,7 +1473,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1483,13 +1484,13 @@
         <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F18" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1499,7 +1500,7 @@
         <v>1.35</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1510,13 +1511,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F19" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1526,7 +1527,7 @@
         <v>0.52</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1537,13 +1538,13 @@
         <v>3</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F20" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1553,7 +1554,7 @@
         <v>0.25</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1567,7 +1568,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>4</v>
@@ -1580,7 +1581,7 @@
         <v>7.92</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1591,13 +1592,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F22" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1607,7 +1608,7 @@
         <v>1.4</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1618,13 +1619,13 @@
         <v>15</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F23" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1634,7 +1635,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1645,13 +1646,13 @@
         <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="E24" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F24" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1661,7 +1662,7 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1672,13 +1673,13 @@
         <v>17</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E25" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F25" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1688,7 +1689,7 @@
         <v>0.61</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1696,16 +1697,16 @@
         <v>8</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="E26" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F26" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1715,7 +1716,7 @@
         <v>0.254</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1726,13 +1727,13 @@
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F27" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1742,7 +1743,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1753,13 +1754,13 @@
         <v>14</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>50</v>
+        <v>179</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F28" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1769,7 +1770,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1780,13 +1781,13 @@
         <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F29" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1796,7 +1797,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1807,13 +1808,13 @@
         <v>9</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F30" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1823,7 +1824,7 @@
         <v>0.66600000000000004</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1834,21 +1835,19 @@
         <v>9</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G31" s="11">
         <v>0.998</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1862,37 +1861,37 @@
         <v>23</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F32" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G32" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="E33" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F33" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1902,7 +1901,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1913,23 +1912,23 @@
         <v>13</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>25</v>
+        <v>177</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F34" s="7">
+        <v>109</v>
+      </c>
+      <c r="F34" s="12">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G34" s="11">
-        <v>8.9999999999999993E-3</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1937,26 +1936,26 @@
         <v>10</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>154</v>
+        <v>25</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="F35" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G35" s="11">
-        <v>1.35</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>161</v>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1964,23 +1963,23 @@
         <v>10</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F36" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G36" s="11">
-        <v>0.66600000000000004</v>
+        <v>1.35</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>158</v>
@@ -1991,26 +1990,26 @@
         <v>10</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="F37" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G37" s="11">
-        <v>5.35</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2018,26 +2017,26 @@
         <v>10</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>118</v>
+        <v>41</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F38" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G38" s="11">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>119</v>
+        <v>5.35</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2045,26 +2044,26 @@
         <v>10</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="F39" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G39" s="11">
-        <v>0.189</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2072,26 +2071,26 @@
         <v>10</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F40" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G40" s="11">
-        <v>3.0000000000000001E-3</v>
+        <v>0.189</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2102,23 +2101,23 @@
         <v>14</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F41" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G41" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2129,13 +2128,13 @@
         <v>14</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F42" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -2145,7 +2144,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2156,23 +2155,23 @@
         <v>14</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F43" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G43" s="11">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2183,40 +2182,40 @@
         <v>14</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="F44" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G44" s="11">
-        <v>3.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="F45" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -2226,138 +2225,165 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>155</v>
+        <v>18</v>
       </c>
       <c r="F46" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G46" s="11">
-        <v>1.52</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>160</v>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>18</v>
+        <v>104</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="F47" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47" s="11">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1.52</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>126</v>
+        <v>18</v>
       </c>
       <c r="F48" s="7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G48" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F49" s="7">
+        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
+        <v>1</v>
+      </c>
+      <c r="G49" s="11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F49" s="7">
-        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>1</v>
-      </c>
-      <c r="G49" s="11">
+      <c r="C50" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F50" s="7">
+        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
+        <v>1</v>
+      </c>
+      <c r="G50" s="11">
         <v>7.13</v>
       </c>
-      <c r="H49" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="H50" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>6</v>
       </c>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50" s="4"/>
-      <c r="E50"/>
-      <c r="F50" s="7">
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51" s="4"/>
+      <c r="E51"/>
+      <c r="F51" s="7">
         <f>SUBTOTAL(109,Table3[Quantity])</f>
-        <v>105</v>
-      </c>
-      <c r="G50" s="11">
+        <v>103</v>
+      </c>
+      <c r="G51" s="11">
         <f>SUMPRODUCT(Table3[Quantity],Table3[Unit Price])</f>
-        <v>41.210000000000008</v>
-      </c>
-      <c r="H50"/>
+        <v>39.26400000000001</v>
+      </c>
+      <c r="H51"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H45" r:id="rId1" xr:uid="{EE7DF417-10AE-4E70-A810-62405DBF25B5}"/>
+    <hyperlink ref="H46" r:id="rId1" xr:uid="{EE7DF417-10AE-4E70-A810-62405DBF25B5}"/>
     <hyperlink ref="H32" r:id="rId2" xr:uid="{66F23E1B-C082-4EC6-9CC9-2C171418CB5E}"/>
     <hyperlink ref="H2" r:id="rId3" xr:uid="{66F23E1B-C082-4EC6-9CC9-2C171418CB5E}"/>
     <hyperlink ref="H12" r:id="rId4" xr:uid="{66F23E1B-C082-4EC6-9CC9-2C171418CB5E}"/>
@@ -2373,42 +2399,43 @@
     <hyperlink ref="H15" r:id="rId14" xr:uid="{D82E1FAC-B21E-4D0C-8072-B74E23C35500}"/>
     <hyperlink ref="H17" r:id="rId15" xr:uid="{4A97A4B3-8886-413E-A5C2-E046B6AEFB80}"/>
     <hyperlink ref="H22" r:id="rId16" xr:uid="{78F79284-D377-49CD-BB85-0D6D27D19393}"/>
-    <hyperlink ref="H38" r:id="rId17" xr:uid="{56849559-98AA-4D22-AF55-F68E96B00DCA}"/>
+    <hyperlink ref="H39" r:id="rId17" xr:uid="{56849559-98AA-4D22-AF55-F68E96B00DCA}"/>
     <hyperlink ref="H23" r:id="rId18" xr:uid="{161C245E-49EC-42EB-B876-97E747F6B253}"/>
     <hyperlink ref="H24" r:id="rId19" xr:uid="{6F901656-AA5E-4379-BC0A-239F12728B6D}"/>
     <hyperlink ref="H27" r:id="rId20" xr:uid="{04358139-6557-4892-86EF-65BA453F8493}"/>
     <hyperlink ref="H28" r:id="rId21" xr:uid="{F0EF2171-794C-46F1-9F62-9E050F5E22FA}"/>
     <hyperlink ref="H29" r:id="rId22" xr:uid="{D2F19171-1397-4C7F-A16B-3ADF2B9E41E3}"/>
     <hyperlink ref="H33" r:id="rId23" xr:uid="{7B7C8CBD-B91C-49E5-9BC0-0285B1908C21}"/>
-    <hyperlink ref="H34" r:id="rId24" xr:uid="{3E5AEFD4-4FEE-474C-9F33-12B4FD71F95A}"/>
-    <hyperlink ref="H39" r:id="rId25" xr:uid="{032EC3F8-9993-4CBE-B683-63BFA82930DC}"/>
-    <hyperlink ref="H40" r:id="rId26" xr:uid="{88C53276-9250-429F-8B02-7B2144F5DBED}"/>
-    <hyperlink ref="H41" r:id="rId27" xr:uid="{D4979280-758F-4B06-92B2-94ED6617EA3D}"/>
-    <hyperlink ref="H42" r:id="rId28" xr:uid="{1AFA7CCD-E8CE-4020-BB62-9DC174DB63D9}"/>
-    <hyperlink ref="H43" r:id="rId29" xr:uid="{18D05616-0CC9-4704-A5DE-2D8CAA5FB28C}"/>
-    <hyperlink ref="H44" r:id="rId30" xr:uid="{4D2DF5C5-FAC2-47E1-91C3-EC5156CD6CCB}"/>
-    <hyperlink ref="H47" r:id="rId31" xr:uid="{171F1A85-C7C4-4C67-B74F-280618700EB9}"/>
-    <hyperlink ref="H48" r:id="rId32" xr:uid="{13B9CC28-DB84-408A-9EFC-D841F0B9A86C}"/>
+    <hyperlink ref="H35" r:id="rId24" xr:uid="{3E5AEFD4-4FEE-474C-9F33-12B4FD71F95A}"/>
+    <hyperlink ref="H40" r:id="rId25" xr:uid="{032EC3F8-9993-4CBE-B683-63BFA82930DC}"/>
+    <hyperlink ref="H41" r:id="rId26" xr:uid="{88C53276-9250-429F-8B02-7B2144F5DBED}"/>
+    <hyperlink ref="H42" r:id="rId27" xr:uid="{D4979280-758F-4B06-92B2-94ED6617EA3D}"/>
+    <hyperlink ref="H43" r:id="rId28" xr:uid="{1AFA7CCD-E8CE-4020-BB62-9DC174DB63D9}"/>
+    <hyperlink ref="H44" r:id="rId29" xr:uid="{18D05616-0CC9-4704-A5DE-2D8CAA5FB28C}"/>
+    <hyperlink ref="H45" r:id="rId30" xr:uid="{4D2DF5C5-FAC2-47E1-91C3-EC5156CD6CCB}"/>
+    <hyperlink ref="H48" r:id="rId31" xr:uid="{171F1A85-C7C4-4C67-B74F-280618700EB9}"/>
+    <hyperlink ref="H49" r:id="rId32" xr:uid="{13B9CC28-DB84-408A-9EFC-D841F0B9A86C}"/>
     <hyperlink ref="H26" r:id="rId33" xr:uid="{C9C2B7A2-0308-4011-BF23-EF457733E8A7}"/>
     <hyperlink ref="H7" r:id="rId34" xr:uid="{C986D14B-A744-43DB-AFE3-103B8CA2C9C1}"/>
-    <hyperlink ref="H36" r:id="rId35" xr:uid="{8F2E8885-742F-4D7E-870D-B0FCAACB139A}"/>
-    <hyperlink ref="H46" r:id="rId36" xr:uid="{B60CF34A-4DD0-47F8-A772-E5FCDC332D1A}"/>
-    <hyperlink ref="H35" r:id="rId37" xr:uid="{EA29696C-72AD-4D50-99DB-D2E6EC2C8852}"/>
+    <hyperlink ref="H37" r:id="rId35" xr:uid="{8F2E8885-742F-4D7E-870D-B0FCAACB139A}"/>
+    <hyperlink ref="H47" r:id="rId36" xr:uid="{B60CF34A-4DD0-47F8-A772-E5FCDC332D1A}"/>
+    <hyperlink ref="H36" r:id="rId37" xr:uid="{EA29696C-72AD-4D50-99DB-D2E6EC2C8852}"/>
     <hyperlink ref="H18" r:id="rId38" xr:uid="{C2920BB8-2CD1-4038-8110-9D23B0D7FA5E}"/>
     <hyperlink ref="H19" r:id="rId39" xr:uid="{98AD1D05-131D-4C33-92FF-AA46F064669E}"/>
     <hyperlink ref="H9" r:id="rId40" xr:uid="{44F7D19E-5926-436C-B35B-58B454AFC995}"/>
     <hyperlink ref="H21" r:id="rId41" xr:uid="{1442176B-A8B1-4F16-8EBF-C1D1DB7291E0}"/>
-    <hyperlink ref="H49" r:id="rId42" xr:uid="{706F3C5B-7E58-4CCF-B1D8-99B733C0152E}"/>
-    <hyperlink ref="H37" r:id="rId43" xr:uid="{B1FDB2F0-B64F-4C13-95CA-87D2B33D853B}"/>
+    <hyperlink ref="H50" r:id="rId42" xr:uid="{706F3C5B-7E58-4CCF-B1D8-99B733C0152E}"/>
+    <hyperlink ref="H38" r:id="rId43" xr:uid="{B1FDB2F0-B64F-4C13-95CA-87D2B33D853B}"/>
     <hyperlink ref="H20" r:id="rId44" xr:uid="{62909AF7-36AF-4DC2-A356-AE4072CDFDCD}"/>
     <hyperlink ref="H8" r:id="rId45" xr:uid="{16C89A90-38FC-47CE-A39B-B00688823FB5}"/>
     <hyperlink ref="H25" r:id="rId46" xr:uid="{24B1E7AE-EE96-4493-B3DC-1F096C28572F}"/>
     <hyperlink ref="H30" r:id="rId47" xr:uid="{D56B83DF-92C5-4D39-9F2E-EBCF911DA34E}"/>
+    <hyperlink ref="H34" r:id="rId48" xr:uid="{33B88EFC-C501-4B9B-9958-552262E7B2BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId48"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId49"/>
   <tableParts count="1">
-    <tablePart r:id="rId49"/>
+    <tablePart r:id="rId50"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PCB revision 1.3 with USB Type-C, more datasheets
</commit_message>
<xml_diff>
--- a/pcb/BOM.xlsx
+++ b/pcb/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design\Nosumor\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F353BAD-CF8A-4E5E-96EA-0638FC2F87AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4559D91B-80A7-499A-AF35-CF9BF3CECCF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28665" yWindow="105" windowWidth="22530" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30015" yWindow="14190" windowWidth="22530" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="181">
   <si>
     <t>Type</t>
   </si>
@@ -156,15 +156,9 @@
     <t>USB3370B</t>
   </si>
   <si>
-    <t>U3</t>
-  </si>
-  <si>
     <t>20k</t>
   </si>
   <si>
-    <t>L3</t>
-  </si>
-  <si>
     <t>J4</t>
   </si>
   <si>
@@ -285,15 +279,9 @@
     <t>2u2</t>
   </si>
   <si>
-    <t>C40, C41, C42, C46, C49, C51, C52</t>
-  </si>
-  <si>
     <t>C50</t>
   </si>
   <si>
-    <t>C39, C47</t>
-  </si>
-  <si>
     <t>U8</t>
   </si>
   <si>
@@ -309,33 +297,12 @@
     <t>R28</t>
   </si>
   <si>
-    <t>R15, R16, R17, R18, R19</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
     <t>4u7</t>
   </si>
   <si>
-    <t>C5, C6</t>
-  </si>
-  <si>
-    <t>C28, C30</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
     <t>Q2</t>
   </si>
   <si>
-    <t>C27, C29, C31, C32, C33, C36, C37, C48</t>
-  </si>
-  <si>
     <t>D4, D5</t>
   </si>
   <si>
@@ -345,18 +312,9 @@
     <t>Q3, Q4, Q5, Q6</t>
   </si>
   <si>
-    <t>R12, R13, R14</t>
-  </si>
-  <si>
-    <t>C1, C4, C34, C35, C38, C43, C44, C45</t>
-  </si>
-  <si>
     <t>K1, K2</t>
   </si>
   <si>
-    <t>R10, R11, R21, R22, R23, R24, R25, R26</t>
-  </si>
-  <si>
     <t>FT2232H</t>
   </si>
   <si>
@@ -544,6 +502,78 @@
   </si>
   <si>
     <t>https://www.mouser.co.uk/ProductDetail/611-KSC623JLFG</t>
+  </si>
+  <si>
+    <t>C41, C48</t>
+  </si>
+  <si>
+    <t>C42, C43, C44, C51, C53, C54, C55</t>
+  </si>
+  <si>
+    <t>U3, U7</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>R16, R17, R18, R19, R20</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>C5, C6, C29, C38</t>
+  </si>
+  <si>
+    <t>C1, C4, C35, C36, C40, C45, C46, C47</t>
+  </si>
+  <si>
+    <t>C27, C30, C32, C33, C34, C37, C39, C49, C52</t>
+  </si>
+  <si>
+    <t>C28, C31</t>
+  </si>
+  <si>
+    <t>USB Type-C</t>
+  </si>
+  <si>
+    <t>R10, R12, R22, R23, R24, R25, R26, R27</t>
+  </si>
+  <si>
+    <t>R13, R14, R15</t>
+  </si>
+  <si>
+    <t>5k1</t>
+  </si>
+  <si>
+    <t>R31, R32</t>
+  </si>
+  <si>
+    <t>RC0402FR-075K1L</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/603-RC0402FR-075K1L</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>R11, R30</t>
+  </si>
+  <si>
+    <t>RC0402FR-070RL</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/603-RC0402FR-070RL</t>
+  </si>
+  <si>
+    <t>CX90M-16P</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/798-CX90M-16P</t>
   </si>
 </sst>
 </file>
@@ -651,10 +681,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A4B88EC-684F-4D5A-8F53-23ADBD7DDE28}" name="Table3" displayName="Table3" ref="A1:H50" totalsRowCount="1" headerRowDxfId="9">
-  <autoFilter ref="A1:H49" xr:uid="{C6C29A0C-1C9D-4BBE-AA50-69AB5F03B3F7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H49">
-    <sortCondition ref="A1:A49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A4B88EC-684F-4D5A-8F53-23ADBD7DDE28}" name="Table3" displayName="Table3" ref="A1:H51" totalsRowCount="1" headerRowDxfId="9">
+  <autoFilter ref="A1:H50" xr:uid="{C6C29A0C-1C9D-4BBE-AA50-69AB5F03B3F7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H50">
+    <sortCondition ref="A1:A50"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{52C12E02-52FF-4249-B643-36E1BF14DE4D}" name="Section" totalsRowLabel="Total" dataDxfId="8"/>
@@ -971,11 +1001,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1040,7 @@
         <v>20</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -1027,10 +1057,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="F2">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1040,7 +1070,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1054,10 +1084,10 @@
         <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1067,7 +1097,7 @@
         <v>0.218</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1078,13 +1108,13 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="F4">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1094,7 +1124,7 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1105,23 +1135,23 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>95</v>
+        <v>164</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="F5" s="6">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G5" s="5">
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1132,13 +1162,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F6">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1148,7 +1178,7 @@
         <v>0.81599999999999995</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1159,23 +1189,23 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>159</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F7">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="5">
         <v>0.25</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1186,13 +1216,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>87</v>
+        <v>160</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F8">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1202,7 +1232,7 @@
         <v>8.5299999999999994</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1210,26 +1240,26 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>176</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9">
-        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>1</v>
+        <v>177</v>
+      </c>
+      <c r="F9" s="6">
+        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
+        <v>2</v>
       </c>
       <c r="G9" s="5">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>148</v>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1240,13 +1270,13 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="F10">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1256,7 +1286,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1267,13 +1297,13 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>92</v>
+        <v>161</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F11">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1283,7 +1313,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1294,13 +1324,13 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="F12">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1310,7 +1340,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1324,20 +1354,20 @@
         <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>100</v>
+        <v>166</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="F13">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G13" s="5">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1351,10 +1381,10 @@
         <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>96</v>
+        <v>167</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F14">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1364,7 +1394,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1375,13 +1405,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>105</v>
+        <v>165</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="F15">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1391,7 +1421,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1402,23 +1432,23 @@
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>168</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
       <c r="F16">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G16" s="5">
-        <v>1.65</v>
+        <v>1.75</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1432,10 +1462,10 @@
         <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F17">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1445,7 +1475,7 @@
         <v>0.46100000000000002</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1462,7 +1492,7 @@
         <v>24</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F18">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1472,7 +1502,7 @@
         <v>0.25</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1483,7 +1513,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>39</v>
@@ -1499,7 +1529,7 @@
         <v>7.9</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1513,10 +1543,10 @@
         <v>40</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F20">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1526,7 +1556,7 @@
         <v>1.21</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1540,10 +1570,10 @@
         <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F21">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1553,7 +1583,7 @@
         <v>0.27400000000000002</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1567,10 +1597,10 @@
         <v>28</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="F22">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1580,7 +1610,7 @@
         <v>0.67300000000000004</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1594,10 +1624,10 @@
         <v>30</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F23">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1607,7 +1637,7 @@
         <v>0.23</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1618,13 +1648,13 @@
         <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="F24">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1634,7 +1664,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1648,10 +1678,10 @@
         <v>23</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>107</v>
+        <v>169</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F25">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1661,7 +1691,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1672,13 +1702,13 @@
         <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F26">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1688,7 +1718,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1699,13 +1729,13 @@
         <v>13</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F27" s="6">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -1715,7 +1745,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1723,20 +1753,26 @@
         <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>34</v>
+        <v>171</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28">
+        <v>172</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="6">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>2</v>
       </c>
       <c r="G28" s="5">
-        <v>1</v>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1747,50 +1783,44 @@
         <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="F29">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29" s="5">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>170</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="F30">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G30" s="5">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>152</v>
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1801,20 +1831,20 @@
         <v>12</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>137</v>
       </c>
       <c r="F31">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G31" s="5">
-        <v>0.1</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>138</v>
@@ -1828,23 +1858,23 @@
         <v>12</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F32">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G32" s="5">
-        <v>6.6000000000000003E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1852,26 +1882,26 @@
         <v>10</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F33">
+        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>5</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33">
-        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>1</v>
-      </c>
       <c r="G33" s="5">
-        <v>1.65</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>162</v>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1879,26 +1909,26 @@
         <v>10</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>135</v>
+        <v>72</v>
       </c>
       <c r="F34">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G34" s="5">
-        <v>0.58699999999999997</v>
+        <v>1.65</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1906,26 +1936,26 @@
         <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F35" s="6">
+        <v>121</v>
+      </c>
+      <c r="F35">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G35" s="5">
-        <v>0.25</v>
+        <v>0.58699999999999997</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>167</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1936,23 +1966,23 @@
         <v>3</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>108</v>
+        <v>37</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F36">
+        <v>77</v>
+      </c>
+      <c r="F36" s="6">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G36" s="5">
-        <v>4.43</v>
+        <v>0.25</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1960,26 +1990,26 @@
         <v>10</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>112</v>
+        <v>38</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="F37">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37" s="5">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>148</v>
+        <v>4.43</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1987,26 +2017,26 @@
         <v>10</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
       <c r="F38">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G38" s="5">
-        <v>0.67300000000000004</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2014,26 +2044,26 @@
         <v>10</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="F39">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G39" s="5">
-        <v>3.0000000000000001E-3</v>
+        <v>0.67300000000000004</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2044,13 +2074,13 @@
         <v>13</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>149</v>
+        <v>66</v>
       </c>
       <c r="F40">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -2060,7 +2090,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>150</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2071,13 +2101,13 @@
         <v>13</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="F41">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
@@ -2087,7 +2117,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2098,283 +2128,311 @@
         <v>13</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F42">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G42" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F43" s="6">
-        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="F43">
+        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
+        <v>4</v>
       </c>
       <c r="G43" s="5">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>152</v>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>131</v>
+        <v>21</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F44" s="6">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G44" s="5">
-        <v>0.35099999999999998</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F45">
+        <v>118</v>
+      </c>
+      <c r="F45" s="6">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G45" s="5">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>152</v>
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F46">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G46" s="5">
-        <v>6.6000000000000003E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="F47">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
         <v>1</v>
       </c>
       <c r="G47" s="5">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>164</v>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>151</v>
+        <v>73</v>
       </c>
       <c r="F48">
         <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G48" s="5">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>152</v>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F49">
+        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
+        <v>4</v>
+      </c>
+      <c r="G49" s="5">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F49">
-        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
-        <v>1</v>
-      </c>
-      <c r="G49" s="5">
+      <c r="C50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F50">
+        <f>IF(LEN(TRIM(Table3[Designator]))=0,0,LEN(TRIM(Table3[Designator]))-LEN(SUBSTITUTE(Table3[Designator],",",""))+1)</f>
+        <v>1</v>
+      </c>
+      <c r="G50" s="5">
         <v>7.13</v>
       </c>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>6</v>
       </c>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50" s="2"/>
-      <c r="E50"/>
-      <c r="F50">
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51" s="2"/>
+      <c r="E51"/>
+      <c r="F51">
         <f>SUBTOTAL(109,Table3[Quantity])</f>
-        <v>112</v>
-      </c>
-      <c r="G50" s="5">
+        <v>119</v>
+      </c>
+      <c r="G51" s="5">
         <f>SUMPRODUCT(Table3[Quantity],Table3[Unit Price])</f>
-        <v>47.715000000000018</v>
-      </c>
-      <c r="H50"/>
+        <v>48.185000000000016</v>
+      </c>
+      <c r="H51"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H36" r:id="rId1" xr:uid="{E4CD5496-215B-4AAB-98F6-472EA6BD6077}"/>
-    <hyperlink ref="H34" r:id="rId2" xr:uid="{C6CEA2E9-CA3F-45D5-B66E-2233C7F490C9}"/>
-    <hyperlink ref="H31" r:id="rId3" xr:uid="{4C641CE9-BB35-4AC3-93D5-E2291778D088}"/>
+    <hyperlink ref="H37" r:id="rId1" xr:uid="{E4CD5496-215B-4AAB-98F6-472EA6BD6077}"/>
+    <hyperlink ref="H35" r:id="rId2" xr:uid="{C6CEA2E9-CA3F-45D5-B66E-2233C7F490C9}"/>
+    <hyperlink ref="H32" r:id="rId3" xr:uid="{4C641CE9-BB35-4AC3-93D5-E2291778D088}"/>
     <hyperlink ref="H5" r:id="rId4" xr:uid="{6A316ECA-670D-4C34-BC4D-A9E785A43BB3}"/>
     <hyperlink ref="H15" r:id="rId5" xr:uid="{490CA5EF-4F78-4A64-A82C-C8AA45E5577C}"/>
-    <hyperlink ref="H32" r:id="rId6" xr:uid="{CB19F34B-2115-43D6-9E35-D04DE9CA5EED}"/>
-    <hyperlink ref="H46" r:id="rId7" xr:uid="{10AF60D7-45C7-4307-B735-30FEDB469480}"/>
+    <hyperlink ref="H33" r:id="rId6" xr:uid="{CB19F34B-2115-43D6-9E35-D04DE9CA5EED}"/>
+    <hyperlink ref="H47" r:id="rId7" xr:uid="{10AF60D7-45C7-4307-B735-30FEDB469480}"/>
     <hyperlink ref="H19" r:id="rId8" xr:uid="{BD2A74C9-59FF-4FE8-BCC2-4B72153B9F6A}"/>
     <hyperlink ref="H22" r:id="rId9" xr:uid="{5E8002F3-4177-47A8-B01B-600B96D991CF}"/>
-    <hyperlink ref="H38" r:id="rId10" xr:uid="{F38B4018-04B8-4DD7-BD30-C32D7477BFB9}"/>
+    <hyperlink ref="H39" r:id="rId10" xr:uid="{F38B4018-04B8-4DD7-BD30-C32D7477BFB9}"/>
     <hyperlink ref="H8" r:id="rId11" xr:uid="{5161A874-4546-4CA2-8AE3-CC3A7F8CCD5F}"/>
-    <hyperlink ref="H44" r:id="rId12" xr:uid="{E76753F6-CC27-4A8F-AF0C-102CE52C4F49}"/>
-    <hyperlink ref="H9" r:id="rId13" xr:uid="{39A7BB8A-9CE8-4BC4-93D7-96DB8FA58ED4}"/>
-    <hyperlink ref="H37" r:id="rId14" xr:uid="{C80B9647-79D6-4364-94DA-3B949E69BA38}"/>
-    <hyperlink ref="H40" r:id="rId15" xr:uid="{427A1ADB-7D9F-4199-A277-D0E8395353F1}"/>
-    <hyperlink ref="H13" r:id="rId16" xr:uid="{A6D6D26F-FC47-405B-B6FE-B0135BC98149}"/>
-    <hyperlink ref="H2" r:id="rId17" xr:uid="{302A3B45-9335-4E5B-841F-1F98FC4F4D08}"/>
-    <hyperlink ref="H30" r:id="rId18" xr:uid="{FD593368-2966-4C38-BF92-6782D2C5B49A}"/>
-    <hyperlink ref="H43" r:id="rId19" xr:uid="{EDDE5802-C73A-4EFC-9518-A51F4B0A4D76}"/>
-    <hyperlink ref="H45" r:id="rId20" xr:uid="{1976E5DA-3348-4FC3-865A-61DCF829CA98}"/>
-    <hyperlink ref="H48" r:id="rId21" xr:uid="{85A5F5BD-3495-49B3-A66D-581D010986FC}"/>
-    <hyperlink ref="H24" r:id="rId22" xr:uid="{9EDC22C3-D733-4F85-B9E4-47FCD040A951}"/>
-    <hyperlink ref="H23" r:id="rId23" xr:uid="{446E7C32-7997-458F-8C48-73CE87EB39C8}"/>
-    <hyperlink ref="H11" r:id="rId24" xr:uid="{AC0DCE45-2558-4E5A-AE06-51F062AD8DE6}"/>
-    <hyperlink ref="H4" r:id="rId25" xr:uid="{4AA5C5FB-7866-430E-9ADA-D1AF0E6B0B58}"/>
-    <hyperlink ref="H12" r:id="rId26" xr:uid="{84879796-791D-41F1-AA16-4F0188F15508}"/>
-    <hyperlink ref="H16" r:id="rId27" xr:uid="{D6314F7C-A13F-43C9-8D77-0426273A2E80}"/>
-    <hyperlink ref="H33" r:id="rId28" xr:uid="{25993CF2-E57D-4001-92E4-4A5BAB0C70E3}"/>
-    <hyperlink ref="H6" r:id="rId29" xr:uid="{AA054B9F-95BC-4754-808E-9151589CD18D}"/>
-    <hyperlink ref="H47" r:id="rId30" xr:uid="{2924F1AA-25E2-4360-A410-F1182415418E}"/>
-    <hyperlink ref="H3" r:id="rId31" xr:uid="{047F635A-DA4D-468F-9A2C-A2BF9A9AAD79}"/>
-    <hyperlink ref="H14" r:id="rId32" xr:uid="{256D4AC2-5A21-4F75-8849-4C0B96CF1264}"/>
-    <hyperlink ref="H17" r:id="rId33" xr:uid="{F3075CF6-A32A-425A-B45E-DAE0AAB6E3F0}"/>
-    <hyperlink ref="H7" r:id="rId34" xr:uid="{0BE27D6F-6D70-4AA8-811E-D48517BDAD55}"/>
-    <hyperlink ref="H18" r:id="rId35" xr:uid="{D2FD08C1-A311-4952-AE2B-4FA648995564}"/>
-    <hyperlink ref="H35" r:id="rId36" xr:uid="{E7449CAD-82B9-43C5-8D35-1C15F9204D7A}"/>
-    <hyperlink ref="H20" r:id="rId37" xr:uid="{0801DB1A-0B29-49DB-ACFE-8F2E1F46B277}"/>
-    <hyperlink ref="H21" r:id="rId38" xr:uid="{C9281895-C07D-4C9F-A52D-53114C952D49}"/>
-    <hyperlink ref="H25" r:id="rId39" xr:uid="{95470E7B-1DC5-4765-95B0-652CF7036AB9}"/>
-    <hyperlink ref="H39" r:id="rId40" xr:uid="{08796A3F-FF8C-4255-805A-3EFC828A82DA}"/>
-    <hyperlink ref="H10" r:id="rId41" xr:uid="{837D2487-34EB-42BD-8F7E-17C4C96925A0}"/>
-    <hyperlink ref="H26" r:id="rId42" xr:uid="{6DC9B30E-33BA-4E78-B6FD-E12CD8160AF0}"/>
-    <hyperlink ref="H27" r:id="rId43" xr:uid="{5B446032-0097-4212-88FF-A46425070825}"/>
-    <hyperlink ref="H41" r:id="rId44" xr:uid="{10072EA1-39DF-4887-86C3-86E59E24D74B}"/>
-    <hyperlink ref="H42" r:id="rId45" xr:uid="{1B7ECA84-95A6-4781-B222-291C9281385C}"/>
-    <hyperlink ref="H29" r:id="rId46" xr:uid="{18F4BCC4-9DDB-461F-96B1-8912B33AD643}"/>
+    <hyperlink ref="H45" r:id="rId12" xr:uid="{E76753F6-CC27-4A8F-AF0C-102CE52C4F49}"/>
+    <hyperlink ref="H38" r:id="rId13" xr:uid="{C80B9647-79D6-4364-94DA-3B949E69BA38}"/>
+    <hyperlink ref="H41" r:id="rId14" xr:uid="{427A1ADB-7D9F-4199-A277-D0E8395353F1}"/>
+    <hyperlink ref="H13" r:id="rId15" xr:uid="{A6D6D26F-FC47-405B-B6FE-B0135BC98149}"/>
+    <hyperlink ref="H2" r:id="rId16" xr:uid="{302A3B45-9335-4E5B-841F-1F98FC4F4D08}"/>
+    <hyperlink ref="H31" r:id="rId17" xr:uid="{FD593368-2966-4C38-BF92-6782D2C5B49A}"/>
+    <hyperlink ref="H44" r:id="rId18" xr:uid="{EDDE5802-C73A-4EFC-9518-A51F4B0A4D76}"/>
+    <hyperlink ref="H46" r:id="rId19" xr:uid="{1976E5DA-3348-4FC3-865A-61DCF829CA98}"/>
+    <hyperlink ref="H49" r:id="rId20" xr:uid="{85A5F5BD-3495-49B3-A66D-581D010986FC}"/>
+    <hyperlink ref="H24" r:id="rId21" xr:uid="{9EDC22C3-D733-4F85-B9E4-47FCD040A951}"/>
+    <hyperlink ref="H23" r:id="rId22" xr:uid="{446E7C32-7997-458F-8C48-73CE87EB39C8}"/>
+    <hyperlink ref="H11" r:id="rId23" xr:uid="{AC0DCE45-2558-4E5A-AE06-51F062AD8DE6}"/>
+    <hyperlink ref="H4" r:id="rId24" xr:uid="{4AA5C5FB-7866-430E-9ADA-D1AF0E6B0B58}"/>
+    <hyperlink ref="H12" r:id="rId25" xr:uid="{84879796-791D-41F1-AA16-4F0188F15508}"/>
+    <hyperlink ref="H34" r:id="rId26" xr:uid="{25993CF2-E57D-4001-92E4-4A5BAB0C70E3}"/>
+    <hyperlink ref="H6" r:id="rId27" xr:uid="{AA054B9F-95BC-4754-808E-9151589CD18D}"/>
+    <hyperlink ref="H48" r:id="rId28" xr:uid="{2924F1AA-25E2-4360-A410-F1182415418E}"/>
+    <hyperlink ref="H3" r:id="rId29" xr:uid="{047F635A-DA4D-468F-9A2C-A2BF9A9AAD79}"/>
+    <hyperlink ref="H14" r:id="rId30" xr:uid="{256D4AC2-5A21-4F75-8849-4C0B96CF1264}"/>
+    <hyperlink ref="H17" r:id="rId31" xr:uid="{F3075CF6-A32A-425A-B45E-DAE0AAB6E3F0}"/>
+    <hyperlink ref="H7" r:id="rId32" xr:uid="{0BE27D6F-6D70-4AA8-811E-D48517BDAD55}"/>
+    <hyperlink ref="H18" r:id="rId33" xr:uid="{D2FD08C1-A311-4952-AE2B-4FA648995564}"/>
+    <hyperlink ref="H36" r:id="rId34" xr:uid="{E7449CAD-82B9-43C5-8D35-1C15F9204D7A}"/>
+    <hyperlink ref="H20" r:id="rId35" xr:uid="{0801DB1A-0B29-49DB-ACFE-8F2E1F46B277}"/>
+    <hyperlink ref="H21" r:id="rId36" xr:uid="{C9281895-C07D-4C9F-A52D-53114C952D49}"/>
+    <hyperlink ref="H25" r:id="rId37" xr:uid="{95470E7B-1DC5-4765-95B0-652CF7036AB9}"/>
+    <hyperlink ref="H40" r:id="rId38" xr:uid="{08796A3F-FF8C-4255-805A-3EFC828A82DA}"/>
+    <hyperlink ref="H10" r:id="rId39" xr:uid="{837D2487-34EB-42BD-8F7E-17C4C96925A0}"/>
+    <hyperlink ref="H26" r:id="rId40" xr:uid="{6DC9B30E-33BA-4E78-B6FD-E12CD8160AF0}"/>
+    <hyperlink ref="H27" r:id="rId41" xr:uid="{5B446032-0097-4212-88FF-A46425070825}"/>
+    <hyperlink ref="H42" r:id="rId42" xr:uid="{10072EA1-39DF-4887-86C3-86E59E24D74B}"/>
+    <hyperlink ref="H43" r:id="rId43" xr:uid="{1B7ECA84-95A6-4781-B222-291C9281385C}"/>
+    <hyperlink ref="H30" r:id="rId44" xr:uid="{18F4BCC4-9DDB-461F-96B1-8912B33AD643}"/>
+    <hyperlink ref="H28" r:id="rId45" xr:uid="{FCAEED36-1076-42F0-A2BB-A63E436C3D23}"/>
+    <hyperlink ref="H9" r:id="rId46" xr:uid="{A0570EE1-3C04-4A87-99D1-A6B7E9672B9F}"/>
+    <hyperlink ref="H16" r:id="rId47" xr:uid="{AB64DF6B-DC25-4829-8DC6-93DA91FD1316}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId48"/>
   <tableParts count="1">
-    <tablePart r:id="rId48"/>
+    <tablePart r:id="rId49"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>